<commit_message>
Adding enhancements for W6.1 - Hass Avocado Dashboard - Part 2: Demonstration
</commit_message>
<xml_diff>
--- a/Area Geocode.xlsx
+++ b/Area Geocode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ensign College\BA_280\LDSBC_BA280_DA_cp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23526A8-7129-48E3-949D-7FA13F137BC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3EC2C1-C0BA-4025-B7D8-E575C8E0AD66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6976A3C-F8B0-4232-B273-96AEA32D8D24}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="165">
   <si>
     <t>region</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Wyoming</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>NH</t>
   </si>
   <si>
@@ -529,24 +526,22 @@
     <t>city</t>
   </si>
   <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area </t>
+    <t> -86.6813</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="170" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,13 +561,6 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -595,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -603,7 +591,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99C874C-BD79-4E7B-88B7-909180357C79}">
   <dimension ref="A1:S1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B46" activeCellId="2" sqref="B32 B33 B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,56 +933,63 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
         <v>157</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>158</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>159</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>161</v>
       </c>
-      <c r="F1" t="s">
-        <v>162</v>
-      </c>
       <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
         <v>73</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="F2">
+        <v>66952</v>
+      </c>
+      <c r="G2" s="4">
+        <v>39.809699999999999</v>
+      </c>
+      <c r="H2" s="4">
+        <v>-98.555599999999998</v>
+      </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -999,28 +998,34 @@
         <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="F3" s="8">
+        <v>35242</v>
+      </c>
+      <c r="G3" s="4">
+        <v>33.416600000000003</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4">
         <v>85001</v>
@@ -1047,10 +1052,17 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="F5">
+        <v>93501</v>
+      </c>
+      <c r="G5" s="7">
+        <v>35.043999999999997</v>
+      </c>
+      <c r="H5" s="2">
+        <v>-118.2527</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1058,16 +1070,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6">
         <v>90001</v>
@@ -1085,16 +1097,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7">
         <v>94203</v>
@@ -1112,16 +1124,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8">
         <v>92101</v>
@@ -1139,16 +1151,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9">
         <v>94101</v>
@@ -1163,19 +1175,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10">
         <v>80201</v>
@@ -1190,19 +1202,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11">
         <v>6101</v>
@@ -1217,19 +1229,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12">
         <v>32099</v>
@@ -1244,19 +1256,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13">
         <v>33101</v>
@@ -1271,19 +1283,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="6">
         <v>32801</v>
@@ -1298,19 +1310,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15">
         <v>33601</v>
@@ -1325,19 +1337,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16">
         <v>30301</v>
@@ -1352,19 +1364,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F17">
         <v>83701</v>
@@ -1385,13 +1397,13 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
         <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F18">
         <v>60601</v>
@@ -1412,13 +1424,13 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19">
         <v>46201</v>
@@ -1433,10 +1445,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>0</v>
@@ -1445,26 +1457,34 @@
         <v>33</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="F20">
+        <v>66012</v>
+      </c>
+      <c r="G20">
+        <v>39.115499999999997</v>
+      </c>
+      <c r="H20" s="4">
+        <v>-94.626800000000003</v>
+      </c>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21">
         <v>40201</v>
@@ -1479,19 +1499,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D22" t="s">
         <v>35</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F22">
         <v>70112</v>
@@ -1506,19 +1526,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D23" t="s">
         <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23">
         <v>2101</v>
@@ -1533,19 +1553,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24" t="s">
         <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F24">
         <v>21201</v>
@@ -1560,10 +1580,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
         <v>121</v>
-      </c>
-      <c r="B25" t="s">
-        <v>122</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>0</v>
@@ -1572,10 +1592,17 @@
         <v>37</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="F25">
+        <v>20602</v>
+      </c>
+      <c r="G25" s="4">
+        <v>39.0458</v>
+      </c>
+      <c r="H25" s="4">
+        <v>-76.641300000000001</v>
+      </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1586,13 +1613,13 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D26" t="s">
         <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F26">
         <v>48201</v>
@@ -1613,13 +1640,13 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s">
         <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F27">
         <v>49588</v>
@@ -1646,27 +1673,34 @@
         <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="F28">
+        <v>48003</v>
+      </c>
+      <c r="G28" s="4">
+        <v>44.314799999999998</v>
+      </c>
+      <c r="H28" s="4">
+        <v>-85.602400000000003</v>
+      </c>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D29" t="s">
         <v>41</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F29">
         <v>63101</v>
@@ -1681,19 +1715,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D30" t="s">
         <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30">
         <v>28201</v>
@@ -1708,19 +1742,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F31">
         <v>27561</v>
@@ -1735,59 +1769,73 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>165</v>
+        <v>135</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>47</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="F32">
+        <v>3862</v>
+      </c>
+      <c r="G32" s="4">
+        <v>43.193899999999999</v>
+      </c>
+      <c r="H32" s="4">
+        <v>-71.572400000000002</v>
+      </c>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="B33" t="s">
-        <v>156</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>166</v>
+        <v>155</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>49</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="F33">
+        <v>87105</v>
+      </c>
+      <c r="G33" s="4">
+        <v>34.5199</v>
+      </c>
+      <c r="H33" s="4">
+        <v>-105.87009999999999</v>
+      </c>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" t="s">
         <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F34">
         <v>89101</v>
@@ -1802,19 +1850,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D35" t="s">
         <v>51</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35">
         <v>12201</v>
@@ -1829,19 +1877,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
         <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36">
         <v>14201</v>
@@ -1856,19 +1904,19 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F37">
         <v>10001</v>
@@ -1883,19 +1931,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
         <v>51</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F38">
         <v>13201</v>
@@ -1916,13 +1964,13 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D39" t="s">
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F39">
         <v>45201</v>
@@ -1943,13 +1991,13 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D40" t="s">
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F40">
         <v>43085</v>
@@ -1964,10 +2012,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>0</v>
@@ -1976,27 +2024,34 @@
         <v>53</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
+        <v>104</v>
+      </c>
+      <c r="F41">
+        <v>73008</v>
+      </c>
+      <c r="G41" s="4">
+        <v>35.467599999999997</v>
+      </c>
+      <c r="H41" s="4">
+        <v>-97.516400000000004</v>
+      </c>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
         <v>54</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F42">
         <v>97201</v>
@@ -2011,19 +2066,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D43" t="s">
         <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F43">
         <v>17101</v>
@@ -2038,19 +2093,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D44" t="s">
         <v>55</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F44">
         <v>19019</v>
@@ -2065,19 +2120,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D45" t="s">
         <v>55</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45">
         <v>15201</v>
@@ -2092,30 +2147,37 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>68</v>
+        <v>148</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>57</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
+        <v>107</v>
+      </c>
+      <c r="F46">
+        <v>29414</v>
+      </c>
+      <c r="G46" s="4">
+        <v>33.836100000000002</v>
+      </c>
+      <c r="H46" s="4">
+        <v>-81.163700000000006</v>
+      </c>
       <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>0</v>
@@ -2124,27 +2186,34 @@
         <v>59</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="F47">
+        <v>37011</v>
+      </c>
+      <c r="G47" s="4">
+        <v>35.517499999999998</v>
+      </c>
+      <c r="H47" s="4">
+        <v>-86.580399999999997</v>
+      </c>
       <c r="I47" s="4"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D48" t="s">
         <v>59</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F48">
         <v>37201</v>
@@ -2159,19 +2228,19 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D49" t="s">
         <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F49">
         <v>75201</v>
@@ -2186,19 +2255,19 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
         <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F50">
         <v>77000</v>
@@ -2213,10 +2282,10 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>0</v>
@@ -2225,7 +2294,10 @@
         <v>61</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="F51">
+        <v>84044</v>
       </c>
       <c r="G51" s="4">
         <v>39.320999999999998</v>
@@ -2237,19 +2309,19 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
         <v>62</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F52">
         <v>23201</v>
@@ -2264,19 +2336,19 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D53" t="s">
         <v>62</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F53">
         <v>24001</v>
@@ -2291,19 +2363,19 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D54" t="s">
         <v>64</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F54">
         <v>98060</v>
@@ -2318,19 +2390,19 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
         <v>64</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F55" s="6">
         <v>99201</v>
@@ -8995,7 +9067,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -9006,10 +9078,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -9020,10 +9092,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -9034,10 +9106,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -9048,10 +9120,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
@@ -9062,10 +9134,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
@@ -9076,10 +9148,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -9090,10 +9162,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -9104,10 +9176,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
@@ -9118,10 +9190,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
         <v>57</v>
@@ -9132,10 +9204,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
         <v>59</v>
@@ -9146,10 +9218,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>62</v>
@@ -9160,10 +9232,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -9174,10 +9246,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -9188,10 +9260,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -9202,10 +9274,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -9216,10 +9288,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -9230,10 +9302,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
@@ -9244,10 +9316,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
         <v>48</v>
@@ -9258,10 +9330,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>55</v>
@@ -9272,10 +9344,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
         <v>56</v>
@@ -9286,10 +9358,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
         <v>63</v>
@@ -9300,10 +9372,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
         <v>66</v>
@@ -9314,10 +9386,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
@@ -9328,10 +9400,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -9342,10 +9414,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
@@ -9356,10 +9428,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
         <v>40</v>
@@ -9370,10 +9442,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
@@ -9384,10 +9456,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
@@ -9398,10 +9470,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
         <v>46</v>
@@ -9412,10 +9484,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
@@ -9426,10 +9498,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
@@ -9440,10 +9512,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
@@ -9454,10 +9526,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
         <v>53</v>
@@ -9468,10 +9540,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
         <v>60</v>
@@ -9482,10 +9554,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
         <v>21</v>
@@ -9496,10 +9568,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
@@ -9510,10 +9582,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>28</v>
@@ -9524,10 +9596,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
         <v>42</v>
@@ -9538,10 +9610,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
         <v>126</v>
-      </c>
-      <c r="B40" t="s">
-        <v>127</v>
       </c>
       <c r="D40">
         <v>9</v>
@@ -9549,10 +9621,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -9563,10 +9635,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -9577,10 +9649,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
         <v>30</v>
@@ -9591,10 +9663,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
         <v>43</v>
@@ -9605,10 +9677,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
         <v>49</v>
@@ -9619,10 +9691,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" t="s">
         <v>50</v>
@@ -9633,10 +9705,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C47" t="s">
         <v>54</v>
@@ -9647,10 +9719,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C48" t="s">
         <v>61</v>
@@ -9661,10 +9733,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
         <v>64</v>
@@ -9675,10 +9747,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
         <v>67</v>

</xml_diff>